<commit_message>
Fix expansion for year_vtg dimension
</commit_message>
<xml_diff>
--- a/message_ix/tools/add_tech/tech_data.xlsx
+++ b/message_ix/tools/add_tech/tech_data.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="inv_cost" sheetId="1" r:id="rId1"/>
-    <sheet name="fix_cost" sheetId="2" r:id="rId2"/>
-    <sheet name="var_cost" sheetId="3" r:id="rId3"/>
+    <sheet name="technical_lifetime" sheetId="1" r:id="rId1"/>
+    <sheet name="inv_cost" sheetId="2" r:id="rId2"/>
+    <sheet name="initial_new_capacity_up" sheetId="3" r:id="rId3"/>
+    <sheet name="growth_new_capacity_up" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
   <si>
     <t>node_loc</t>
   </si>
@@ -42,25 +43,16 @@
     <t>DACCS</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>$/kW</t>
   </si>
   <si>
-    <t>year_act</t>
-  </si>
-  <si>
-    <t>$/kWa</t>
-  </si>
-  <si>
-    <t>mode</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
-    <t>y</t>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -418,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,8 +440,11 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
       <c r="D2">
-        <v>2500</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -457,15 +452,86 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>710</v>
+      </c>
       <c r="D3">
-        <v>2200</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -476,13 +542,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,41 +559,112 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="C3">
+        <v>710</v>
+      </c>
+      <c r="D3">
+        <v>1496.842348095947</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>896.2148060213547</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>1197.473878476757</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>716.9718448170837</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -537,13 +674,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,59 +691,244 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>710</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>710</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest update of prototyping
</commit_message>
<xml_diff>
--- a/message_ix/tools/add_tech/tech_data.xlsx
+++ b/message_ix/tools/add_tech/tech_data.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="technical_lifetime" sheetId="1" r:id="rId1"/>
-    <sheet name="inv_cost" sheetId="2" r:id="rId2"/>
-    <sheet name="initial_new_capacity_up" sheetId="3" r:id="rId3"/>
-    <sheet name="growth_new_capacity_up" sheetId="4" r:id="rId4"/>
+    <sheet name="inv_cost" sheetId="1" r:id="rId1"/>
+    <sheet name="initial_new_capacity_up" sheetId="2" r:id="rId2"/>
+    <sheet name="fix_cost" sheetId="3" r:id="rId3"/>
+    <sheet name="technical_lifetime" sheetId="4" r:id="rId4"/>
+    <sheet name="growth_new_capacity_up" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="14">
   <si>
     <t>node_loc</t>
   </si>
@@ -43,13 +44,19 @@
     <t>DACCS</t>
   </si>
   <si>
+    <t>$/kW</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>year_act</t>
+  </si>
+  <si>
+    <t>$/kWa</t>
+  </si>
+  <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>$/kW</t>
-  </si>
-  <si>
-    <t>GW</t>
   </si>
   <si>
     <t>-</t>
@@ -444,7 +451,7 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -461,7 +468,7 @@
         <v>710</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>1496.842348095947</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -478,7 +485,7 @@
         <v>720</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>896.2148060213547</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -495,7 +502,7 @@
         <v>700</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -512,7 +519,7 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>1197.473878476757</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -529,7 +536,7 @@
         <v>720</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>716.9718448170838</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -576,7 +583,7 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>2500</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -593,7 +600,7 @@
         <v>710</v>
       </c>
       <c r="D3">
-        <v>1496.842348095947</v>
+        <v>0.5</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -610,7 +617,7 @@
         <v>720</v>
       </c>
       <c r="D4">
-        <v>896.2148060213547</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -627,7 +634,7 @@
         <v>700</v>
       </c>
       <c r="D5">
-        <v>2000</v>
+        <v>0.5</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -644,7 +651,7 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>1197.473878476757</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -661,7 +668,7 @@
         <v>720</v>
       </c>
       <c r="D7">
-        <v>716.9718448170837</v>
+        <v>0.5</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -674,13 +681,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,13 +698,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -708,13 +718,16 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -722,16 +735,19 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3" t="s">
+        <v>710</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -739,35 +755,41 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4" t="s">
+        <v>720</v>
+      </c>
+      <c r="E4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5" t="s">
+        <v>710</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -776,15 +798,18 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
-      </c>
-      <c r="E6" t="s">
+        <v>720</v>
+      </c>
+      <c r="E6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -793,10 +818,133 @@
         <v>720</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7" t="s">
+        <v>720</v>
+      </c>
+      <c r="E7">
         <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="D8">
+        <v>700</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>710</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>700</v>
+      </c>
+      <c r="D10">
+        <v>720</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>710</v>
+      </c>
+      <c r="D11">
+        <v>710</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>710</v>
+      </c>
+      <c r="D12">
+        <v>720</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>720</v>
+      </c>
+      <c r="D13">
+        <v>720</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -840,10 +988,10 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -857,10 +1005,10 @@
         <v>710</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -874,10 +1022,10 @@
         <v>720</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -891,10 +1039,10 @@
         <v>700</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -908,10 +1056,10 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -925,10 +1073,142 @@
         <v>720</v>
       </c>
       <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
         <v>0.5</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>710</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all expansion except input and output
</commit_message>
<xml_diff>
--- a/message_ix/tools/add_tech/tech_data.xlsx
+++ b/message_ix/tools/add_tech/tech_data.xlsx
@@ -7,18 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="inv_cost" sheetId="1" r:id="rId1"/>
-    <sheet name="initial_new_capacity_up" sheetId="2" r:id="rId2"/>
-    <sheet name="fix_cost" sheetId="3" r:id="rId3"/>
+    <sheet name="initial_new_capacity_up" sheetId="1" r:id="rId1"/>
+    <sheet name="emission_factor" sheetId="2" r:id="rId2"/>
+    <sheet name="var_cost" sheetId="3" r:id="rId3"/>
     <sheet name="technical_lifetime" sheetId="4" r:id="rId4"/>
     <sheet name="growth_new_capacity_up" sheetId="5" r:id="rId5"/>
+    <sheet name="fix_cost" sheetId="6" r:id="rId6"/>
+    <sheet name="capacity_factor" sheetId="7" r:id="rId7"/>
+    <sheet name="inv_cost" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="22">
   <si>
     <t>node_loc</t>
   </si>
@@ -44,13 +47,34 @@
     <t>DACCS</t>
   </si>
   <si>
-    <t>$/kW</t>
-  </si>
-  <si>
     <t>GW</t>
   </si>
   <si>
     <t>year_act</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>emission</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>tCO2/kWa</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
   <si>
     <t>$/kWa</t>
@@ -60,6 +84,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>$/kW</t>
   </si>
 </sst>
 </file>
@@ -451,7 +478,7 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>2500</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -468,7 +495,7 @@
         <v>710</v>
       </c>
       <c r="D3">
-        <v>1496.842348095947</v>
+        <v>0.5</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -485,7 +512,7 @@
         <v>720</v>
       </c>
       <c r="D4">
-        <v>896.2148060213547</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -502,7 +529,7 @@
         <v>700</v>
       </c>
       <c r="D5">
-        <v>2000</v>
+        <v>0.5</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -519,7 +546,7 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>1197.473878476757</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -536,7 +563,7 @@
         <v>720</v>
       </c>
       <c r="D7">
-        <v>716.9718448170838</v>
+        <v>0.5</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -549,13 +576,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,13 +593,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -583,13 +619,22 @@
         <v>700</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>700</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>-20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -597,16 +642,25 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>710</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>-20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -614,35 +668,53 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>720</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>-20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>710</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>-20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -651,15 +723,24 @@
         <v>710</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>720</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>-20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -668,10 +749,487 @@
         <v>720</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>720</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>-20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="D8">
+        <v>700</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>710</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>700</v>
+      </c>
+      <c r="D10">
+        <v>720</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>710</v>
+      </c>
+      <c r="D11">
+        <v>710</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>710</v>
+      </c>
+      <c r="D12">
+        <v>720</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>720</v>
+      </c>
+      <c r="D13">
+        <v>720</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>700</v>
+      </c>
+      <c r="D14">
+        <v>700</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>-20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>700</v>
+      </c>
+      <c r="D15">
+        <v>710</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>-20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>700</v>
+      </c>
+      <c r="D16">
+        <v>720</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>-20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>710</v>
+      </c>
+      <c r="D17">
+        <v>710</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>-20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>710</v>
+      </c>
+      <c r="D18">
+        <v>720</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>-20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>720</v>
+      </c>
+      <c r="D19">
+        <v>720</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>-20</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>700</v>
+      </c>
+      <c r="D20">
+        <v>700</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>700</v>
+      </c>
+      <c r="D21">
+        <v>710</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>700</v>
+      </c>
+      <c r="D22">
+        <v>720</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>710</v>
+      </c>
+      <c r="D23">
+        <v>710</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>710</v>
+      </c>
+      <c r="D24">
+        <v>720</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>720</v>
+      </c>
+      <c r="D25">
+        <v>720</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -681,13 +1239,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,16 +1256,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -720,14 +1284,20 @@
       <c r="D2">
         <v>700</v>
       </c>
-      <c r="E2">
-        <v>10</v>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -740,14 +1310,20 @@
       <c r="D3">
         <v>710</v>
       </c>
-      <c r="E3">
-        <v>10</v>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>134.3916379344122</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -760,14 +1336,20 @@
       <c r="D4">
         <v>720</v>
       </c>
-      <c r="E4">
-        <v>10</v>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>180.6111234669415</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -780,14 +1362,20 @@
       <c r="D5">
         <v>710</v>
       </c>
-      <c r="E5">
-        <v>10</v>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>59.87369392383787</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -800,14 +1388,20 @@
       <c r="D6">
         <v>720</v>
       </c>
-      <c r="E6">
-        <v>10</v>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>80.46523795608236</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -820,14 +1414,20 @@
       <c r="D7">
         <v>720</v>
       </c>
-      <c r="E7">
-        <v>10</v>
+      <c r="E7" t="s">
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>35.84859224085419</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -840,14 +1440,20 @@
       <c r="D8">
         <v>700</v>
       </c>
-      <c r="E8">
-        <v>10</v>
+      <c r="E8" t="s">
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>80</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -860,14 +1466,20 @@
       <c r="D9">
         <v>710</v>
       </c>
-      <c r="E9">
-        <v>10</v>
+      <c r="E9" t="s">
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>107.5133103475298</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -880,14 +1492,20 @@
       <c r="D10">
         <v>720</v>
       </c>
-      <c r="E10">
-        <v>10</v>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>144.4888987735532</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -900,14 +1518,20 @@
       <c r="D11">
         <v>710</v>
       </c>
-      <c r="E11">
-        <v>10</v>
+      <c r="E11" t="s">
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G11">
+        <v>47.8989551390703</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -920,14 +1544,20 @@
       <c r="D12">
         <v>720</v>
       </c>
-      <c r="E12">
-        <v>10</v>
+      <c r="E12" t="s">
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>64.37219036486589</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -940,11 +1570,17 @@
       <c r="D13">
         <v>720</v>
       </c>
-      <c r="E13">
-        <v>10</v>
+      <c r="E13" t="s">
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>28.67887379268335</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1627,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1008,7 +1644,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1025,7 +1661,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1042,7 +1678,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1059,7 +1695,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1076,7 +1712,7 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1759,7 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1140,7 +1776,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1157,7 +1793,7 @@
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1174,7 +1810,7 @@
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1191,7 +1827,7 @@
         <v>0.5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1208,7 +1844,724 @@
         <v>0.5</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>700</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+      <c r="D3">
+        <v>710</v>
+      </c>
+      <c r="E3">
+        <v>13.43916379344122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>700</v>
+      </c>
+      <c r="D4">
+        <v>720</v>
+      </c>
+      <c r="E4">
+        <v>18.06111234669415</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>710</v>
+      </c>
+      <c r="D5">
+        <v>710</v>
+      </c>
+      <c r="E5">
+        <v>5.987369392383787</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>720</v>
+      </c>
+      <c r="E6">
+        <v>8.046523795608236</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>720</v>
+      </c>
+      <c r="E7">
+        <v>3.584859224085419</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="D8">
+        <v>700</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>710</v>
+      </c>
+      <c r="E9">
+        <v>10.75133103475298</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>700</v>
+      </c>
+      <c r="D10">
+        <v>720</v>
+      </c>
+      <c r="E10">
+        <v>14.44888987735532</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>710</v>
+      </c>
+      <c r="D11">
+        <v>710</v>
+      </c>
+      <c r="E11">
+        <v>4.78989551390703</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>710</v>
+      </c>
+      <c r="D12">
+        <v>720</v>
+      </c>
+      <c r="E12">
+        <v>6.437219036486589</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>720</v>
+      </c>
+      <c r="D13">
+        <v>720</v>
+      </c>
+      <c r="E13">
+        <v>2.867887379268335</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>700</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+      <c r="D3">
+        <v>710</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>700</v>
+      </c>
+      <c r="D4">
+        <v>720</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>710</v>
+      </c>
+      <c r="D5">
+        <v>710</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>720</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>720</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="D8">
+        <v>700</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>710</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>700</v>
+      </c>
+      <c r="D10">
+        <v>720</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>710</v>
+      </c>
+      <c r="D11">
+        <v>710</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>710</v>
+      </c>
+      <c r="D12">
+        <v>720</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>720</v>
+      </c>
+      <c r="D13">
+        <v>720</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>700</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>710</v>
+      </c>
+      <c r="D3">
+        <v>1496.842348095947</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>720</v>
+      </c>
+      <c r="D4">
+        <v>896.2148060213547</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>1197.473878476757</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>716.9718448170838</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>